<commit_message>
MOZ: TAS update forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/sn_lf_pretas_1_sites_202007.xlsx
+++ b/LF/PreTAS/Senegal/sn_lf_pretas_1_sites_202007.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Senegal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517EB829-2A6B-441C-B887-416A2A47A6E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DB4AE-A6CB-44F0-BFF5-4FE3E06154FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -338,12 +338,6 @@
     <t>Selon les groupes d'âge ciblés, combien de participants admissibles sont présents dans cette école ou communauté ?</t>
   </si>
   <si>
-    <t>(Septembre 2020) 1. Pre-TAS FL - Formulaire Site</t>
-  </si>
-  <si>
-    <t>sn_lf_pretas_1_sites_202009</t>
-  </si>
-  <si>
     <t>L'école ou la communauté (à travers le directeur et l'APE ou le chef de lacommunauté) consent-elle à participer à cette enquête ?</t>
   </si>
   <si>
@@ -555,6 +549,12 @@
   </si>
   <si>
     <t>select_one code_site_list</t>
+  </si>
+  <si>
+    <t>(Septembre 2020) 1. Pre-TAS FL - Formulaire Site V2</t>
+  </si>
+  <si>
+    <t>sn_lf_pretas_1_sites_202009_v2</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1211,17 +1211,17 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>94</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12"/>
@@ -1236,22 +1236,22 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
@@ -1272,7 +1272,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="8"/>
@@ -1339,11 +1339,11 @@
         <v>21</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="14"/>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G44" sqref="G44:G71"/>
     </sheetView>
   </sheetViews>
@@ -1563,7 +1563,7 @@
         <v>93</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1778,16 +1778,16 @@
     </row>
     <row r="16" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>76</v>
@@ -1798,16 +1798,16 @@
     </row>
     <row r="17" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>82</v>
@@ -1818,16 +1818,16 @@
     </row>
     <row r="18" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E18" s="34" t="s">
         <v>82</v>
@@ -1838,16 +1838,16 @@
     </row>
     <row r="19" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E19" s="34" t="s">
         <v>78</v>
@@ -1858,16 +1858,16 @@
     </row>
     <row r="20" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>77</v>
@@ -1878,16 +1878,16 @@
     </row>
     <row r="21" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>84</v>
@@ -1898,16 +1898,16 @@
     </row>
     <row r="22" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>81</v>
@@ -1918,16 +1918,16 @@
     </row>
     <row r="23" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E23" s="34" t="s">
         <v>80</v>
@@ -1938,16 +1938,16 @@
     </row>
     <row r="24" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E24" s="34" t="s">
         <v>89</v>
@@ -1958,16 +1958,16 @@
     </row>
     <row r="25" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>79</v>
@@ -1978,16 +1978,16 @@
     </row>
     <row r="26" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E26" s="34" t="s">
         <v>84</v>
@@ -1998,16 +1998,16 @@
     </row>
     <row r="27" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>77</v>
@@ -2018,16 +2018,16 @@
     </row>
     <row r="28" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>81</v>
@@ -2038,16 +2038,16 @@
     </row>
     <row r="29" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="34" t="s">
         <v>87</v>
@@ -2058,16 +2058,16 @@
     </row>
     <row r="30" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E30" s="34" t="s">
         <v>85</v>
@@ -2078,16 +2078,16 @@
     </row>
     <row r="31" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E31" s="34" t="s">
         <v>88</v>
@@ -2098,16 +2098,16 @@
     </row>
     <row r="32" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E32" s="34" t="s">
         <v>85</v>
@@ -2118,16 +2118,16 @@
     </row>
     <row r="33" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E33" s="34" t="s">
         <v>79</v>
@@ -2138,16 +2138,16 @@
     </row>
     <row r="34" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E34" s="34" t="s">
         <v>83</v>
@@ -2158,16 +2158,16 @@
     </row>
     <row r="35" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E35" s="34" t="s">
         <v>76</v>
@@ -2178,16 +2178,16 @@
     </row>
     <row r="36" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E36" s="34" t="s">
         <v>87</v>
@@ -2198,16 +2198,16 @@
     </row>
     <row r="37" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E37" s="34" t="s">
         <v>78</v>
@@ -2218,16 +2218,16 @@
     </row>
     <row r="38" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E38" s="34" t="s">
         <v>86</v>
@@ -2238,16 +2238,16 @@
     </row>
     <row r="39" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E39" s="34" t="s">
         <v>83</v>
@@ -2258,16 +2258,16 @@
     </row>
     <row r="40" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E40" s="34" t="s">
         <v>86</v>
@@ -2278,16 +2278,16 @@
     </row>
     <row r="41" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E41" s="34" t="s">
         <v>80</v>
@@ -2298,16 +2298,16 @@
     </row>
     <row r="42" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E42" s="34" t="s">
         <v>88</v>
@@ -2318,16 +2318,16 @@
     </row>
     <row r="43" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E43" s="34" t="s">
         <v>89</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="44" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B44" s="33">
         <v>101</v>
@@ -2351,12 +2351,12 @@
       </c>
       <c r="E44" s="35"/>
       <c r="G44" s="36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B45" s="33">
         <v>102</v>
@@ -2369,12 +2369,12 @@
       </c>
       <c r="E45" s="35"/>
       <c r="G45" s="36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B46" s="33">
         <v>103</v>
@@ -2387,12 +2387,12 @@
       </c>
       <c r="E46" s="35"/>
       <c r="G46" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B47" s="33">
         <v>104</v>
@@ -2405,12 +2405,12 @@
       </c>
       <c r="E47" s="35"/>
       <c r="G47" s="36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B48" s="33">
         <v>105</v>
@@ -2423,12 +2423,12 @@
       </c>
       <c r="E48" s="35"/>
       <c r="G48" s="36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B49" s="33">
         <v>106</v>
@@ -2441,12 +2441,12 @@
       </c>
       <c r="E49" s="35"/>
       <c r="G49" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B50" s="33">
         <v>107</v>
@@ -2459,12 +2459,12 @@
       </c>
       <c r="E50" s="35"/>
       <c r="G50" s="36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B51" s="33">
         <v>108</v>
@@ -2477,12 +2477,12 @@
       </c>
       <c r="E51" s="35"/>
       <c r="G51" s="36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B52" s="33">
         <v>109</v>
@@ -2495,12 +2495,12 @@
       </c>
       <c r="E52" s="35"/>
       <c r="G52" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B53" s="33">
         <v>110</v>
@@ -2513,12 +2513,12 @@
       </c>
       <c r="E53" s="35"/>
       <c r="G53" s="36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B54" s="33">
         <v>111</v>
@@ -2531,12 +2531,12 @@
       </c>
       <c r="E54" s="35"/>
       <c r="G54" s="36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B55" s="33">
         <v>112</v>
@@ -2549,12 +2549,12 @@
       </c>
       <c r="E55" s="35"/>
       <c r="G55" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B56" s="33">
         <v>113</v>
@@ -2567,12 +2567,12 @@
       </c>
       <c r="E56" s="35"/>
       <c r="G56" s="36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B57" s="33">
         <v>114</v>
@@ -2585,12 +2585,12 @@
       </c>
       <c r="E57" s="35"/>
       <c r="G57" s="36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B58" s="33">
         <v>115</v>
@@ -2603,12 +2603,12 @@
       </c>
       <c r="E58" s="35"/>
       <c r="G58" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B59" s="33">
         <v>116</v>
@@ -2621,12 +2621,12 @@
       </c>
       <c r="E59" s="35"/>
       <c r="G59" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B60" s="33">
         <v>117</v>
@@ -2639,12 +2639,12 @@
       </c>
       <c r="E60" s="35"/>
       <c r="G60" s="36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B61" s="33">
         <v>118</v>
@@ -2657,12 +2657,12 @@
       </c>
       <c r="E61" s="35"/>
       <c r="G61" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B62" s="33">
         <v>119</v>
@@ -2675,12 +2675,12 @@
       </c>
       <c r="E62" s="35"/>
       <c r="G62" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B63" s="33">
         <v>120</v>
@@ -2693,12 +2693,12 @@
       </c>
       <c r="E63" s="35"/>
       <c r="G63" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B64" s="33">
         <v>121</v>
@@ -2711,12 +2711,12 @@
       </c>
       <c r="E64" s="35"/>
       <c r="G64" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B65" s="33">
         <v>122</v>
@@ -2729,12 +2729,12 @@
       </c>
       <c r="E65" s="35"/>
       <c r="G65" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B66" s="33">
         <v>123</v>
@@ -2747,12 +2747,12 @@
       </c>
       <c r="E66" s="35"/>
       <c r="G66" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B67" s="33">
         <v>124</v>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="E67" s="35"/>
       <c r="G67" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B68" s="33">
         <v>125</v>
@@ -2783,12 +2783,12 @@
       </c>
       <c r="E68" s="35"/>
       <c r="G68" s="36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B69" s="33">
         <v>126</v>
@@ -2801,12 +2801,12 @@
       </c>
       <c r="E69" s="35"/>
       <c r="G69" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B70" s="33">
         <v>127</v>
@@ -2819,12 +2819,12 @@
       </c>
       <c r="E70" s="35"/>
       <c r="G70" s="36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" s="33">
         <v>128</v>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="E71" s="35"/>
       <c r="G71" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3235,7 +3235,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -3261,10 +3261,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>174</v>
       </c>
       <c r="C2">
         <v>20200907</v>

</xml_diff>